<commit_message>
book.save seems to be clobbering TABC253.xlsx
</commit_message>
<xml_diff>
--- a/Transactions.xlsx
+++ b/Transactions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!\projects\PycharmProjects\beer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC77F6C-EA5C-45A2-9870-B5AF4E181F8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BDDA7F-DC77-4D81-8F2A-9C07C1D0E45C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="16570" windowHeight="8950" xr2:uid="{B085CBB3-BE45-4267-B265-85ED7EA00774}"/>
   </bookViews>
@@ -424,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{340CA89C-F800-48BA-AE25-071BA324DF40}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -435,6 +435,7 @@
     <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -483,7 +484,7 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>8</v>
+        <v>8.75</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -509,7 +510,7 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>15</v>
+        <v>15.35</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -535,7 +536,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -561,7 +562,7 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>75</v>
+        <v>75.989999999999995</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -587,7 +588,7 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <v>8</v>
+        <v>8.75</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -613,7 +614,7 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>15</v>
+        <v>15.35</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -639,7 +640,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -665,7 +666,7 @@
         <v>1</v>
       </c>
       <c r="G9">
-        <v>8</v>
+        <v>8.75</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -691,7 +692,7 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <v>15</v>
+        <v>15.35</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -717,10 +718,10 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -743,7 +744,7 @@
         <v>1</v>
       </c>
       <c r="G12">
-        <v>8</v>
+        <v>8.75</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -769,10 +770,10 @@
         <v>1</v>
       </c>
       <c r="G13">
-        <v>15</v>
+        <v>15.35</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -795,7 +796,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -821,7 +822,7 @@
         <v>1</v>
       </c>
       <c r="G15">
-        <v>8</v>
+        <v>8.75</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -847,7 +848,7 @@
         <v>1</v>
       </c>
       <c r="G16">
-        <v>8</v>
+        <v>8.75</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -873,7 +874,7 @@
         <v>1</v>
       </c>
       <c r="G17">
-        <v>15</v>
+        <v>15.35</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -899,7 +900,7 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -910,7 +911,7 @@
         <v>44163</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -925,7 +926,7 @@
         <v>1</v>
       </c>
       <c r="G19">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="H19">
         <v>2</v>
@@ -951,7 +952,7 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -977,7 +978,7 @@
         <v>1</v>
       </c>
       <c r="G21">
-        <v>75</v>
+        <v>75.989999999999995</v>
       </c>
       <c r="H21">
         <v>2</v>
@@ -1003,7 +1004,7 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -1029,7 +1030,7 @@
         <v>1</v>
       </c>
       <c r="G23">
-        <v>75</v>
+        <v>75.989999999999995</v>
       </c>
       <c r="H23">
         <v>2</v>
@@ -1055,7 +1056,7 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -1081,7 +1082,7 @@
         <v>1</v>
       </c>
       <c r="G25">
-        <v>75</v>
+        <v>75.989999999999995</v>
       </c>
       <c r="H25">
         <v>2</v>

</xml_diff>